<commit_message>
add: Run experiments on gemini-2.0-flash-exp (prompts N01-N12)
</commit_message>
<xml_diff>
--- a/results/stage1_eval_initial_DR_prompts_126instances/summary_report/level1_avg_metrics_summary.xlsx
+++ b/results/stage1_eval_initial_DR_prompts_126instances/summary_report/level1_avg_metrics_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,12 +504,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[np.float64(0.5729752770673486)]</t>
+          <t>[np.float64(0.5566534914361001), np.float64(0.6381500466818641)]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[0.6587301587301587]</t>
+          <t>[0.6031746031746031, 0.6746031746031746]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -519,14 +519,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>gemini-2.0-flash-exp</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.5729752770673486</v>
+        <v>0.5974017690589821</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6587301587301587</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -535,12 +535,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[np.float64(0.5958838724168912), np.float64(0.5903950216450216)]</t>
+          <t>[np.float64(0.596738572162301), np.float64(0.614869446025248)]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[0.656, 0.6507936507936508]</t>
+          <t>[0.6428571428571429, 0.6507936507936508]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -550,14 +550,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.5931394470309563</v>
+        <v>0.6058040090937744</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6533968253968254</v>
+        <v>0.6468253968253969</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -566,12 +566,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[np.float64(0.5566534914361001), np.float64(0.6381500466818641)]</t>
+          <t>[np.float64(0.5958838724168912), np.float64(0.5903950216450216)]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[0.6031746031746031, 0.6746031746031746]</t>
+          <t>[0.656, 0.6507936507936508]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -581,14 +581,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.5974017690589821</v>
+        <v>0.5931394470309563</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6388888888888888</v>
+        <v>0.6533968253968254</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
@@ -597,12 +597,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[np.float64(0.596738572162301), np.float64(0.614869446025248)]</t>
+          <t>[np.float64(0.5596988795518207), np.float64(0.5581084161646821)]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[0.6428571428571429, 0.6507936507936508]</t>
+          <t>[0.6428571428571429, 0.6428571428571429]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -612,14 +612,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.6058040090937744</v>
+        <v>0.5589036478582514</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6468253968253969</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -628,12 +628,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[np.float64(0.6439088183384013), np.float64(0.6319826907946499)]</t>
+          <t>[np.float64(0.5737225235512418), np.float64(0.5479878201117139)]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[0.6984126984126984, 0.6904761904761905]</t>
+          <t>[0.626984126984127, 0.5952380952380952]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -643,14 +643,14 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.6379457545665256</v>
+        <v>0.5608551718314778</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6944444444444444</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="G7" t="n">
         <v>2</v>
@@ -659,12 +659,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[np.float64(0.5737225235512418), np.float64(0.5479878201117139)]</t>
+          <t>[np.float64(0.6439088183384013), np.float64(0.6319826907946499)]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[0.626984126984127, 0.5952380952380952]</t>
+          <t>[0.6984126984126984, 0.6904761904761905]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -674,14 +674,14 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.5608551718314778</v>
+        <v>0.6379457545665256</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6111111111111112</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="G8" t="n">
         <v>2</v>
@@ -752,43 +752,43 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[np.float64(0.5300044984255511)]</t>
+          <t>[np.float64(0.6291010756919848), np.float64(0.6101042351256586)]</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[0.5555555555555556]</t>
+          <t>[0.6746031746031746, 0.6666666666666666]</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.5300044984255511</v>
+        <v>0.6196026554088216</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.6706349206349207</v>
       </c>
       <c r="G11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[np.float64(0.5708227361741157), np.float64(0.5362849421659832)]</t>
+          <t>[np.float64(0.5300044984255511)]</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[0.6190476190476191, 0.5714285714285714]</t>
+          <t>[0.5555555555555556]</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -798,14 +798,14 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.5535538391700494</v>
+        <v>0.5300044984255511</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5952380952380952</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="G12" t="n">
         <v>3</v>
@@ -814,12 +814,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[np.float64(0.6073608930751787), np.float64(0.5939851114578972)]</t>
+          <t>[np.float64(0.6084540067678396), np.float64(0.586625)]</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[0.664, 0.656]</t>
+          <t>[0.6587301587301587, 0.6428571428571429]</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -829,14 +829,14 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0.600673002266538</v>
+        <v>0.5975395033839197</v>
       </c>
       <c r="F13" t="n">
-        <v>0.66</v>
+        <v>0.6507936507936508</v>
       </c>
       <c r="G13" t="n">
         <v>3</v>
@@ -845,12 +845,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[np.float64(0.6084540067678396), np.float64(0.586625)]</t>
+          <t>[np.float64(0.5708227361741157), np.float64(0.5362849421659832)]</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[0.6587301587301587, 0.6428571428571429]</t>
+          <t>[0.6190476190476191, 0.5714285714285714]</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -860,14 +860,14 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.5975395033839197</v>
+        <v>0.5535538391700494</v>
       </c>
       <c r="F14" t="n">
-        <v>0.6507936507936508</v>
+        <v>0.5952380952380952</v>
       </c>
       <c r="G14" t="n">
         <v>3</v>
@@ -876,74 +876,74 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[np.float64(0.596821360457724), np.float64(0.5975242622301445)]</t>
+          <t>[np.float64(0.6073608930751787), np.float64(0.5939851114578972)]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[0.6587301587301587, 0.6587301587301587]</t>
+          <t>[0.664, 0.656]</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.5971728113439343</v>
+        <v>0.600673002266538</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6587301587301587</v>
+        <v>0.66</v>
       </c>
       <c r="G15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[np.float64(0.5284650630011455)]</t>
+          <t>[np.float64(0.6557137360523279), np.float64(0.6691428349996125)]</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[0.5476190476190477]</t>
+          <t>[0.704, 0.72]</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.5284650630011455</v>
+        <v>0.6624282855259702</v>
       </c>
       <c r="F16" t="n">
-        <v>0.5476190476190477</v>
+        <v>0.712</v>
       </c>
       <c r="G16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>[np.float64(0.6010605883042306), np.float64(0.6109806798728296)]</t>
+          <t>[np.float64(0.596821360457724), np.float64(0.5975242622301445)]</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[0.6666666666666666, 0.6746031746031746]</t>
+          <t>[0.6587301587301587, 0.6587301587301587]</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -953,14 +953,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.6060206340885301</v>
+        <v>0.5971728113439343</v>
       </c>
       <c r="F17" t="n">
-        <v>0.6706349206349207</v>
+        <v>0.6587301587301587</v>
       </c>
       <c r="G17" t="n">
         <v>4</v>
@@ -969,12 +969,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>[np.float64(0.569905501003062), np.float64(0.6138179848954979)]</t>
+          <t>[np.float64(0.5284650630011455)]</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[0.6349206349206349, 0.6746031746031746]</t>
+          <t>[0.5476190476190477]</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -984,14 +984,14 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.59186174294928</v>
+        <v>0.5284650630011455</v>
       </c>
       <c r="F18" t="n">
-        <v>0.6547619047619048</v>
+        <v>0.5476190476190477</v>
       </c>
       <c r="G18" t="n">
         <v>4</v>
@@ -1000,48 +1000,48 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>[np.float64(0.6078249064444157), np.float64(0.6217619143184313)]</t>
+          <t>[np.float64(0.5705309622977199), np.float64(0.5696221959858323)]</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[0.6666666666666666, 0.6825396825396826]</t>
+          <t>[0.6349206349206349, 0.6428571428571429]</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.6147934103814234</v>
+        <v>0.5700765791417761</v>
       </c>
       <c r="F19" t="n">
-        <v>0.6746031746031746</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="G19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>[np.float64(0.688579145205272), np.float64(0.6924327168638965)]</t>
+          <t>[np.float64(0.569905501003062), np.float64(0.6138179848954979)]</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[0.7258064516129032, 0.7235772357723578]</t>
+          <t>[0.6349206349206349, 0.6746031746031746]</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1050,55 +1050,55 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.6905059310345842</v>
+        <v>0.59186174294928</v>
       </c>
       <c r="F20" t="n">
-        <v>0.7246918436926305</v>
+        <v>0.6547619047619048</v>
       </c>
       <c r="G20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>[np.float64(0.507856802131447)]</t>
+          <t>[np.float64(0.6010605883042306), np.float64(0.6109806798728296)]</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[0.5396825396825397]</t>
+          <t>[0.6666666666666666, 0.6746031746031746]</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.507856802131447</v>
+        <v>0.6060206340885301</v>
       </c>
       <c r="F21" t="n">
-        <v>0.5396825396825397</v>
+        <v>0.6706349206349207</v>
       </c>
       <c r="G21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>[np.float64(0.5308119882274092), np.float64(0.5087175936205204)]</t>
+          <t>[np.float64(0.688579145205272), np.float64(0.6924327168638965)]</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[0.6031746031746031, 0.5714285714285714]</t>
+          <t>[0.7258064516129032, 0.7235772357723578]</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1108,14 +1108,14 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.5197647909239648</v>
+        <v>0.6905059310345842</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5873015873015872</v>
+        <v>0.7246918436926305</v>
       </c>
       <c r="G22" t="n">
         <v>5</v>
@@ -1124,110 +1124,110 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>[np.float64(0.5965944667331462)]</t>
+          <t>[np.float64(0.6078249064444157), np.float64(0.6217619143184313)]</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[0.6349206349206349]</t>
+          <t>[0.6666666666666666, 0.6825396825396826]</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.5965944667331462</v>
+        <v>0.6147934103814234</v>
       </c>
       <c r="F23" t="n">
-        <v>0.6349206349206349</v>
+        <v>0.6746031746031746</v>
       </c>
       <c r="G23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>[np.float64(0.6185185185185185), np.float64(0.6535996207182648)]</t>
+          <t>[np.float64(0.507856802131447)]</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[0.6746031746031746, 0.696]</t>
+          <t>[0.5396825396825397]</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0.6360590696183916</v>
+        <v>0.507856802131447</v>
       </c>
       <c r="F24" t="n">
-        <v>0.6853015873015873</v>
+        <v>0.5396825396825397</v>
       </c>
       <c r="G24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>[np.float64(0.647135217723453), np.float64(0.6143999270206167)]</t>
+          <t>[np.float64(0.5937458842370891), np.float64(0.6193183805178909)]</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[0.6935483870967742, 0.664]</t>
+          <t>[0.6587301587301587, 0.6746031746031746]</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.6307675723720348</v>
+        <v>0.6065321323774899</v>
       </c>
       <c r="F25" t="n">
-        <v>0.6787741935483871</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="G25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>[np.float64(0.48113553113553115), np.float64(0.4351327872921321)]</t>
+          <t>[np.float64(0.5308119882274092), np.float64(0.5087175936205204)]</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[0.5238095238095238, 0.48412698412698413]</t>
+          <t>[0.6031746031746031, 0.5714285714285714]</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1236,91 +1236,91 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.4581341592138316</v>
+        <v>0.5197647909239648</v>
       </c>
       <c r="F26" t="n">
-        <v>0.503968253968254</v>
+        <v>0.5873015873015872</v>
       </c>
       <c r="G26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>[np.float64(0.6521265106560312), np.float64(0.6386810592005396)]</t>
+          <t>[np.float64(0.647135217723453), np.float64(0.6143999270206167)]</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[0.6904761904761905, 0.68]</t>
+          <t>[0.6935483870967742, 0.664]</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0.6454037849282854</v>
+        <v>0.6307675723720348</v>
       </c>
       <c r="F27" t="n">
-        <v>0.6852380952380952</v>
+        <v>0.6787741935483871</v>
       </c>
       <c r="G27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>[np.float64(0.5816889632107024), np.float64(0.6205141351605264)]</t>
+          <t>[np.float64(0.6185185185185185), np.float64(0.6535996207182648)]</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[0.6370967741935484, 0.6666666666666666]</t>
+          <t>[0.6746031746031746, 0.696]</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.6011015491856144</v>
+        <v>0.6360590696183916</v>
       </c>
       <c r="F28" t="n">
-        <v>0.6518817204301075</v>
+        <v>0.6853015873015873</v>
       </c>
       <c r="G28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>[np.float64(0.5083562277110025), np.float64(0.5058309297439733)]</t>
+          <t>[np.float64(0.48113553113553115), np.float64(0.4351327872921321)]</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[0.56, 0.552]</t>
+          <t>[0.5238095238095238, 0.48412698412698413]</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1329,91 +1329,91 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0.5070935787274879</v>
+        <v>0.4581341592138316</v>
       </c>
       <c r="F29" t="n">
-        <v>0.556</v>
+        <v>0.503968253968254</v>
       </c>
       <c r="G29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>[np.float64(0.538090032544731)]</t>
+          <t>[np.float64(0.5580430959599905), np.float64(0.5680415979201039)]</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[0.5555555555555556]</t>
+          <t>[0.6111111111111112, 0.626984126984127]</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>0.538090032544731</v>
+        <v>0.5630423469400472</v>
       </c>
       <c r="F30" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="G30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>[np.float64(0.6562992627116154), np.float64(0.6445754716981131)]</t>
+          <t>[np.float64(0.5965944667331462)]</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[0.696, 0.68]</t>
+          <t>[0.6349206349206349]</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0.6504373672048642</v>
+        <v>0.5965944667331462</v>
       </c>
       <c r="F31" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.6349206349206349</v>
       </c>
       <c r="G31" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>[np.float64(0.4541337907375644), np.float64(0.47122859025032937)]</t>
+          <t>[np.float64(0.5083562277110025), np.float64(0.5058309297439733)]</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[0.52, 0.5317460317460317]</t>
+          <t>[0.56, 0.552]</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1422,91 +1422,91 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0.4626811904939468</v>
+        <v>0.5070935787274879</v>
       </c>
       <c r="F32" t="n">
-        <v>0.5258730158730158</v>
+        <v>0.556</v>
       </c>
       <c r="G32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>[np.float64(0.532920304983848)]</t>
+          <t>[np.float64(0.6232943469785575), np.float64(0.5956989247311828)]</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[0.5714285714285714]</t>
+          <t>[0.6666666666666666, 0.6507936507936508]</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0.532920304983848</v>
+        <v>0.6094966358548701</v>
       </c>
       <c r="F33" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.6587301587301587</v>
       </c>
       <c r="G33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>[np.float64(0.6524644518850284), np.float64(0.6482872200263505)]</t>
+          <t>[np.float64(0.538090032544731)]</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[0.7073170731707317, 0.6942148760330579]</t>
+          <t>[0.5555555555555556]</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0.6503758359556895</v>
+        <v>0.538090032544731</v>
       </c>
       <c r="F34" t="n">
-        <v>0.7007659746018948</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="G34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>[np.float64(0.600395721463846), np.float64(0.6682065332823585)]</t>
+          <t>[np.float64(0.5816889632107024), np.float64(0.6205141351605264)]</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[0.6504065040650406, 0.7166666666666667]</t>
+          <t>[0.6370967741935484, 0.6666666666666666]</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1515,60 +1515,60 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0.6343011273731023</v>
+        <v>0.6011015491856144</v>
       </c>
       <c r="F35" t="n">
-        <v>0.6835365853658537</v>
+        <v>0.6518817204301075</v>
       </c>
       <c r="G35" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>[np.float64(0.5361160714285714), np.float64(0.5477406704101712)]</t>
+          <t>[np.float64(0.6521265106560312), np.float64(0.6386810592005396)]</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[0.576, 0.5873015873015873]</t>
+          <t>[0.6904761904761905, 0.68]</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0.5419283709193713</v>
+        <v>0.6454037849282854</v>
       </c>
       <c r="F36" t="n">
-        <v>0.5816507936507936</v>
+        <v>0.6852380952380952</v>
       </c>
       <c r="G36" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>[np.float64(0.5313937481113387)]</t>
+          <t>[np.float64(0.532920304983848)]</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[0.5634920634920635]</t>
+          <t>[0.5714285714285714]</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1577,60 +1577,60 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0.5313937481113387</v>
+        <v>0.532920304983848</v>
       </c>
       <c r="F37" t="n">
-        <v>0.5634920634920635</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>[np.float64(0.6263474048099917), np.float64(0.6086457590876693)]</t>
+          <t>[np.float64(0.6524644518850284), np.float64(0.6482872200263505)]</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[0.6829268292682927, 0.6693548387096774]</t>
+          <t>[0.7073170731707317, 0.6942148760330579]</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0.6174965819488305</v>
+        <v>0.6503758359556895</v>
       </c>
       <c r="F38" t="n">
-        <v>0.6761408339889851</v>
+        <v>0.7007659746018948</v>
       </c>
       <c r="G38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>[np.float64(0.6074765461770609), np.float64(0.5969074715487381)]</t>
+          <t>[np.float64(0.6562992627116154), np.float64(0.6445754716981131)]</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[0.656, 0.6585365853658537]</t>
+          <t>[0.696, 0.68]</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1639,60 +1639,60 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.6021920088628996</v>
+        <v>0.6504373672048642</v>
       </c>
       <c r="F39" t="n">
-        <v>0.6572682926829269</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="G39" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>[np.float64(0.5873665845648604), np.float64(0.5821868173138465)]</t>
+          <t>[np.float64(0.5464676134142537), np.float64(0.5505998448192124)]</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[0.6333333333333333, 0.639344262295082]</t>
+          <t>[0.6031746031746031, 0.6111111111111112]</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0.5847767009393534</v>
+        <v>0.548533729116733</v>
       </c>
       <c r="F40" t="n">
-        <v>0.6363387978142077</v>
+        <v>0.6071428571428572</v>
       </c>
       <c r="G40" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>[np.float64(0.41419540229885055), np.float64(0.3414374445430346)]</t>
+          <t>[np.float64(0.4541337907375644), np.float64(0.47122859025032937)]</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[0.472, 0.4126984126984127]</t>
+          <t>[0.52, 0.5317460317460317]</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1701,60 +1701,60 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0.3778164234209426</v>
+        <v>0.4626811904939468</v>
       </c>
       <c r="F41" t="n">
-        <v>0.4423492063492063</v>
+        <v>0.5258730158730158</v>
       </c>
       <c r="G41" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>[np.float64(0.5447754984853544)]</t>
+          <t>[np.float64(0.600395721463846), np.float64(0.6682065332823585)]</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[0.5793650793650794]</t>
+          <t>[0.6504065040650406, 0.7166666666666667]</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0.5447754984853544</v>
+        <v>0.6343011273731023</v>
       </c>
       <c r="F42" t="n">
-        <v>0.5793650793650794</v>
+        <v>0.6835365853658537</v>
       </c>
       <c r="G42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>[np.float64(0.3380952380952381), np.float64(0.31666666666666665)]</t>
+          <t>[np.float64(0.5361160714285714), np.float64(0.5477406704101712)]</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[0.3333333333333333, 0.38461538461538464]</t>
+          <t>[0.576, 0.5873015873015873]</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1763,167 +1763,508 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.3273809523809524</v>
+        <v>0.5419283709193713</v>
       </c>
       <c r="F43" t="n">
-        <v>0.358974358974359</v>
+        <v>0.5816507936507936</v>
       </c>
       <c r="G43" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>[np.float64(0.5236538107511046), np.float64(0.4968177855274629)]</t>
+          <t>[np.float64(0.6263474048099917), np.float64(0.6086457590876693)]</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[0.5476190476190477, 0.5158730158730159]</t>
+          <t>[0.6829268292682927, 0.6693548387096774]</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0.5102357981392838</v>
+        <v>0.6174965819488305</v>
       </c>
       <c r="F44" t="n">
-        <v>0.5317460317460319</v>
+        <v>0.6761408339889851</v>
       </c>
       <c r="G44" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>[np.float64(0.5237903225806451), np.float64(0.5487336811307223)]</t>
+          <t>[np.float64(0.5313937481113387)]</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[0.5634920634920635, 0.5952380952380952]</t>
+          <t>[0.5634920634920635]</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0.5362620018556836</v>
+        <v>0.5313937481113387</v>
       </c>
       <c r="F45" t="n">
-        <v>0.5793650793650793</v>
+        <v>0.5634920634920635</v>
       </c>
       <c r="G45" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>[np.float64(0.5160615200660967), np.float64(0.5104956066054465)]</t>
+          <t>[np.float64(0.6159932363750098), np.float64(0.5832183782005592)]</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[0.5714285714285714, 0.5634920634920635]</t>
+          <t>[0.6666666666666666, 0.6349206349206349]</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0.5132785633357716</v>
+        <v>0.5996058072877846</v>
       </c>
       <c r="F46" t="n">
-        <v>0.5674603174603174</v>
+        <v>0.6507936507936507</v>
       </c>
       <c r="G46" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>[np.float64(0.48588209656103254), np.float64(0.4766586843438264)]</t>
+          <t>[np.float64(0.6074765461770609), np.float64(0.5969074715487381)]</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[0.5238095238095238, 0.5]</t>
+          <t>[0.656, 0.6585365853658537]</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.4812703904524295</v>
+        <v>0.6021920088628996</v>
       </c>
       <c r="F47" t="n">
-        <v>0.5119047619047619</v>
+        <v>0.6572682926829269</v>
       </c>
       <c r="G47" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
+          <t>[np.float64(0.41419540229885055), np.float64(0.3414374445430346)]</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>[0.472, 0.4126984126984127]</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>promptN10</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>0.3778164234209426</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.4423492063492063</v>
+      </c>
+      <c r="G48" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>[np.float64(0.5203264226500969), np.float64(0.5445767195767196)]</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>[0.5873015873015873, 0.5952380952380952]</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>promptN10</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>gemini-2.0-flash-exp</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>0.5324515711134082</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.5912698412698413</v>
+      </c>
+      <c r="G49" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>[np.float64(0.5873665845648604), np.float64(0.5821868173138465)]</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>[0.6333333333333333, 0.639344262295082]</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>promptN10</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>0.5847767009393534</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.6363387978142077</v>
+      </c>
+      <c r="G50" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>[np.float64(0.5447754984853544)]</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>[0.5793650793650794]</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>promptN10</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>gemini-1.5-flash-001-tuning</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>0.5447754984853544</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.5793650793650794</v>
+      </c>
+      <c r="G51" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>[np.float64(0.3380952380952381), np.float64(0.31666666666666665)]</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>[0.3333333333333333, 0.38461538461538464]</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>0.3273809523809524</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.358974358974359</v>
+      </c>
+      <c r="G52" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>[np.float64(0.5237903225806451), np.float64(0.5487336811307223)]</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>[0.5634920634920635, 0.5952380952380952]</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>0.5362620018556836</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.5793650793650793</v>
+      </c>
+      <c r="G53" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>[np.float64(0.6087991718426502), np.float64(0.5690200322553264)]</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>[0.6428571428571429, 0.6111111111111112]</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>gemini-2.0-flash-exp</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>0.5889096020489883</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.626984126984127</v>
+      </c>
+      <c r="G54" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>[np.float64(0.5236538107511046), np.float64(0.4968177855274629)]</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>[0.5476190476190477, 0.5158730158730159]</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>0.5102357981392838</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.5317460317460319</v>
+      </c>
+      <c r="G55" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
           <t>[np.float64(0.49615630389258436), np.float64(0.508381806163761)]</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B56" t="inlineStr">
         <is>
           <t>[0.5238095238095238, 0.5317460317460317]</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>promptN12</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
-      <c r="E48" t="n">
+      <c r="E56" t="n">
         <v>0.5022690550281728</v>
       </c>
-      <c r="F48" t="n">
+      <c r="F56" t="n">
         <v>0.5277777777777778</v>
       </c>
-      <c r="G48" t="n">
+      <c r="G56" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>[np.float64(0.590716894099558), np.float64(0.5747434017595308)]</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>[0.6428571428571429, 0.6349206349206349]</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>promptN12</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>gemini-2.0-flash-exp</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>0.5827301479295444</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.6388888888888888</v>
+      </c>
+      <c r="G57" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>[np.float64(0.48588209656103254), np.float64(0.4766586843438264)]</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>[0.5238095238095238, 0.5]</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>promptN12</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>0.4812703904524295</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.5119047619047619</v>
+      </c>
+      <c r="G58" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>[np.float64(0.5160615200660967), np.float64(0.5104956066054465)]</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>[0.5714285714285714, 0.5634920634920635]</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>promptN12</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>0.5132785633357716</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.5674603174603174</v>
+      </c>
+      <c r="G59" t="n">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: update evaluation methods to include additional details
</commit_message>
<xml_diff>
--- a/results/stage1_eval_initial_DR_prompts_126instances/summary_report/level1_avg_metrics_summary.xlsx
+++ b/results/stage1_eval_initial_DR_prompts_126instances/summary_report/level1_avg_metrics_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,12 +473,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[np.float64(0.4973336190441453)]</t>
+          <t>[np.float64(0.5566534914361001), np.float64(0.6381500466818641)]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[0.5158730158730159]</t>
+          <t>[0.6031746031746031, 0.6746031746031746]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -488,14 +488,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.4973336190441453</v>
+        <v>0.5974017690589821</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5158730158730159</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -504,12 +504,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[np.float64(0.5566534914361001), np.float64(0.6381500466818641)]</t>
+          <t>[np.float64(0.5965571646634769), np.float64(0.4973336190441453)]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[0.6031746031746031, 0.6746031746031746]</t>
+          <t>[0.6111111111111112, 0.5158730158730159]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -519,14 +519,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-flash-001-finetuned</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.5974017690589821</v>
+        <v>0.5469453918538111</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6388888888888888</v>
+        <v>0.5634920634920635</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -628,12 +628,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[np.float64(0.5737225235512418), np.float64(0.5479878201117139)]</t>
+          <t>[np.float64(0.6051189355006958), np.float64(0.6172799736495389)]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[0.626984126984127, 0.5952380952380952]</t>
+          <t>[0.656, 0.664]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -643,14 +643,14 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.5608551718314778</v>
+        <v>0.6111994545751174</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6111111111111112</v>
+        <v>0.66</v>
       </c>
       <c r="G7" t="n">
         <v>2</v>
@@ -690,12 +690,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[np.float64(0.6051189355006958), np.float64(0.6172799736495389)]</t>
+          <t>[np.float64(0.5737225235512418), np.float64(0.5479878201117139)]</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[0.656, 0.664]</t>
+          <t>[0.626984126984127, 0.5952380952380952]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -705,14 +705,14 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.6111994545751174</v>
+        <v>0.5608551718314778</v>
       </c>
       <c r="F9" t="n">
-        <v>0.66</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="G9" t="n">
         <v>2</v>
@@ -721,12 +721,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[np.float64(0.6077338241717102)]</t>
+          <t>[np.float64(0.630537025698316), np.float64(0.6077338241717102)]</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[0.6349206349206349]</t>
+          <t>[0.648, 0.6349206349206349]</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -736,14 +736,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gemini-1.5-flash-001-finetuned</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.6077338241717102</v>
+        <v>0.6191354249350132</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6349206349206349</v>
+        <v>0.6414603174603175</v>
       </c>
       <c r="G10" t="n">
         <v>2</v>
@@ -783,12 +783,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[np.float64(0.5300044984255511)]</t>
+          <t>[np.float64(0.5708227361741157), np.float64(0.5362849421659832)]</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[0.5555555555555556]</t>
+          <t>[0.6190476190476191, 0.5714285714285714]</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -798,14 +798,14 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.5300044984255511</v>
+        <v>0.5535538391700494</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5952380952380952</v>
       </c>
       <c r="G12" t="n">
         <v>3</v>
@@ -814,12 +814,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[np.float64(0.6084540067678396), np.float64(0.586625)]</t>
+          <t>[np.float64(0.6073608930751787), np.float64(0.5939851114578972)]</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[0.6587301587301587, 0.6428571428571429]</t>
+          <t>[0.664, 0.656]</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -829,14 +829,14 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0.5975395033839197</v>
+        <v>0.600673002266538</v>
       </c>
       <c r="F13" t="n">
-        <v>0.6507936507936508</v>
+        <v>0.66</v>
       </c>
       <c r="G13" t="n">
         <v>3</v>
@@ -845,12 +845,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[np.float64(0.5708227361741157), np.float64(0.5362849421659832)]</t>
+          <t>[np.float64(0.6557137360523279), np.float64(0.6691428349996125)]</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[0.6190476190476191, 0.5714285714285714]</t>
+          <t>[0.704, 0.72]</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -860,14 +860,14 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.5535538391700494</v>
+        <v>0.6624282855259702</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5952380952380952</v>
+        <v>0.712</v>
       </c>
       <c r="G14" t="n">
         <v>3</v>
@@ -876,12 +876,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[np.float64(0.6073608930751787), np.float64(0.5939851114578972)]</t>
+          <t>[np.float64(0.6084540067678396), np.float64(0.586625)]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[0.664, 0.656]</t>
+          <t>[0.6587301587301587, 0.6428571428571429]</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -891,14 +891,14 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.600673002266538</v>
+        <v>0.5975395033839197</v>
       </c>
       <c r="F15" t="n">
-        <v>0.66</v>
+        <v>0.6507936507936508</v>
       </c>
       <c r="G15" t="n">
         <v>3</v>
@@ -907,12 +907,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[np.float64(0.6557137360523279), np.float64(0.6691428349996125)]</t>
+          <t>[np.float64(0.5300044984255511), np.float64(0.5385178047317266)]</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[0.704, 0.72]</t>
+          <t>[0.5555555555555556, 0.5555555555555556]</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -922,14 +922,14 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>gemini-2.0-flash-exp</t>
+          <t>gemini-1.5-flash-001-finetuned</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.6624282855259702</v>
+        <v>0.5342611515786388</v>
       </c>
       <c r="F16" t="n">
-        <v>0.712</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="G16" t="n">
         <v>3</v>
@@ -969,12 +969,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>[np.float64(0.5284650630011455)]</t>
+          <t>[np.float64(0.5221861471861472), np.float64(0.5284650630011455)]</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[0.5476190476190477]</t>
+          <t>[0.5238095238095238, 0.5476190476190477]</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -984,14 +984,14 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gemini-1.5-flash-001-finetuned</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.5284650630011455</v>
+        <v>0.5253256050936463</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5476190476190477</v>
+        <v>0.5357142857142858</v>
       </c>
       <c r="G18" t="n">
         <v>4</v>
@@ -1031,12 +1031,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>[np.float64(0.569905501003062), np.float64(0.6138179848954979)]</t>
+          <t>[np.float64(0.6010605883042306), np.float64(0.6109806798728296)]</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[0.6349206349206349, 0.6746031746031746]</t>
+          <t>[0.6666666666666666, 0.6746031746031746]</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1046,14 +1046,14 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.59186174294928</v>
+        <v>0.6060206340885301</v>
       </c>
       <c r="F20" t="n">
-        <v>0.6547619047619048</v>
+        <v>0.6706349206349207</v>
       </c>
       <c r="G20" t="n">
         <v>4</v>
@@ -1062,12 +1062,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>[np.float64(0.6010605883042306), np.float64(0.6109806798728296)]</t>
+          <t>[np.float64(0.569905501003062), np.float64(0.6138179848954979)]</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[0.6666666666666666, 0.6746031746031746]</t>
+          <t>[0.6349206349206349, 0.6746031746031746]</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1077,14 +1077,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.6060206340885301</v>
+        <v>0.59186174294928</v>
       </c>
       <c r="F21" t="n">
-        <v>0.6706349206349207</v>
+        <v>0.6547619047619048</v>
       </c>
       <c r="G21" t="n">
         <v>4</v>
@@ -1093,12 +1093,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>[np.float64(0.688579145205272), np.float64(0.6924327168638965)]</t>
+          <t>[np.float64(0.507856802131447), np.float64(0.5757882882882883)]</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[0.7258064516129032, 0.7235772357723578]</t>
+          <t>[0.5396825396825397, 0.6031746031746031]</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1108,14 +1108,14 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-flash-001-finetuned</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.6905059310345842</v>
+        <v>0.5418225452098677</v>
       </c>
       <c r="F22" t="n">
-        <v>0.7246918436926305</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G22" t="n">
         <v>5</v>
@@ -1124,12 +1124,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>[np.float64(0.6078249064444157), np.float64(0.6217619143184313)]</t>
+          <t>[np.float64(0.5937458842370891), np.float64(0.6193183805178909)]</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[0.6666666666666666, 0.6825396825396826]</t>
+          <t>[0.6587301587301587, 0.6746031746031746]</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1139,14 +1139,14 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.6147934103814234</v>
+        <v>0.6065321323774899</v>
       </c>
       <c r="F23" t="n">
-        <v>0.6746031746031746</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="G23" t="n">
         <v>5</v>
@@ -1155,12 +1155,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>[np.float64(0.507856802131447)]</t>
+          <t>[np.float64(0.6078249064444157), np.float64(0.6217619143184313)]</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[0.5396825396825397]</t>
+          <t>[0.6666666666666666, 0.6825396825396826]</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1170,14 +1170,14 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0.507856802131447</v>
+        <v>0.6147934103814234</v>
       </c>
       <c r="F24" t="n">
-        <v>0.5396825396825397</v>
+        <v>0.6746031746031746</v>
       </c>
       <c r="G24" t="n">
         <v>5</v>
@@ -1186,12 +1186,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>[np.float64(0.5937458842370891), np.float64(0.6193183805178909)]</t>
+          <t>[np.float64(0.5308119882274092), np.float64(0.5087175936205204)]</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[0.6587301587301587, 0.6746031746031746]</t>
+          <t>[0.6031746031746031, 0.5714285714285714]</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1201,14 +1201,14 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>gemini-2.0-flash-exp</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.6065321323774899</v>
+        <v>0.5197647909239648</v>
       </c>
       <c r="F25" t="n">
-        <v>0.6666666666666667</v>
+        <v>0.5873015873015872</v>
       </c>
       <c r="G25" t="n">
         <v>5</v>
@@ -1217,12 +1217,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>[np.float64(0.5308119882274092), np.float64(0.5087175936205204)]</t>
+          <t>[np.float64(0.688579145205272), np.float64(0.6924327168638965)]</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[0.6031746031746031, 0.5714285714285714]</t>
+          <t>[0.7258064516129032, 0.7235772357723578]</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1232,14 +1232,14 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.5197647909239648</v>
+        <v>0.6905059310345842</v>
       </c>
       <c r="F26" t="n">
-        <v>0.5873015873015872</v>
+        <v>0.7246918436926305</v>
       </c>
       <c r="G26" t="n">
         <v>5</v>
@@ -1248,12 +1248,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>[np.float64(0.647135217723453), np.float64(0.6143999270206167)]</t>
+          <t>[np.float64(0.48113553113553115), np.float64(0.4351327872921321)]</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[0.6935483870967742, 0.664]</t>
+          <t>[0.5238095238095238, 0.48412698412698413]</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1263,14 +1263,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0.6307675723720348</v>
+        <v>0.4581341592138316</v>
       </c>
       <c r="F27" t="n">
-        <v>0.6787741935483871</v>
+        <v>0.503968253968254</v>
       </c>
       <c r="G27" t="n">
         <v>6</v>
@@ -1279,12 +1279,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>[np.float64(0.6185185185185185), np.float64(0.6535996207182648)]</t>
+          <t>[np.float64(0.647135217723453), np.float64(0.6143999270206167)]</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[0.6746031746031746, 0.696]</t>
+          <t>[0.6935483870967742, 0.664]</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1294,14 +1294,14 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.6360590696183916</v>
+        <v>0.6307675723720348</v>
       </c>
       <c r="F28" t="n">
-        <v>0.6853015873015873</v>
+        <v>0.6787741935483871</v>
       </c>
       <c r="G28" t="n">
         <v>6</v>
@@ -1310,12 +1310,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>[np.float64(0.48113553113553115), np.float64(0.4351327872921321)]</t>
+          <t>[np.float64(0.6185185185185185), np.float64(0.6535996207182648)]</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[0.5238095238095238, 0.48412698412698413]</t>
+          <t>[0.6746031746031746, 0.696]</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1325,14 +1325,14 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0.4581341592138316</v>
+        <v>0.6360590696183916</v>
       </c>
       <c r="F29" t="n">
-        <v>0.503968253968254</v>
+        <v>0.6853015873015873</v>
       </c>
       <c r="G29" t="n">
         <v>6</v>
@@ -1341,12 +1341,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>[np.float64(0.5580430959599905), np.float64(0.5680415979201039)]</t>
+          <t>[np.float64(0.5965944667331462), np.float64(0.5729927101070477)]</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[0.6111111111111112, 0.626984126984127]</t>
+          <t>[0.6349206349206349, 0.624]</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1356,14 +1356,14 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>gemini-2.0-flash-exp</t>
+          <t>gemini-1.5-flash-001-finetuned</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>0.5630423469400472</v>
+        <v>0.584793588420097</v>
       </c>
       <c r="F30" t="n">
-        <v>0.6190476190476191</v>
+        <v>0.6294603174603175</v>
       </c>
       <c r="G30" t="n">
         <v>6</v>
@@ -1372,12 +1372,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>[np.float64(0.5965944667331462)]</t>
+          <t>[np.float64(0.5580430959599905), np.float64(0.5680415979201039)]</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[0.6349206349206349]</t>
+          <t>[0.6111111111111112, 0.626984126984127]</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1387,14 +1387,14 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0.5965944667331462</v>
+        <v>0.5630423469400472</v>
       </c>
       <c r="F31" t="n">
-        <v>0.6349206349206349</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="G31" t="n">
         <v>6</v>
@@ -1403,12 +1403,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>[np.float64(0.5083562277110025), np.float64(0.5058309297439733)]</t>
+          <t>[np.float64(0.6232943469785575), np.float64(0.5956989247311828)]</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[0.56, 0.552]</t>
+          <t>[0.6666666666666666, 0.6507936507936508]</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1418,14 +1418,14 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0.5070935787274879</v>
+        <v>0.6094966358548701</v>
       </c>
       <c r="F32" t="n">
-        <v>0.556</v>
+        <v>0.6587301587301587</v>
       </c>
       <c r="G32" t="n">
         <v>7</v>
@@ -1434,12 +1434,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>[np.float64(0.6232943469785575), np.float64(0.5956989247311828)]</t>
+          <t>[np.float64(0.6521265106560312), np.float64(0.6386810592005396)]</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[0.6666666666666666, 0.6507936507936508]</t>
+          <t>[0.6904761904761905, 0.68]</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1449,14 +1449,14 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>gemini-2.0-flash-exp</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0.6094966358548701</v>
+        <v>0.6454037849282854</v>
       </c>
       <c r="F33" t="n">
-        <v>0.6587301587301587</v>
+        <v>0.6852380952380952</v>
       </c>
       <c r="G33" t="n">
         <v>7</v>
@@ -1465,12 +1465,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>[np.float64(0.538090032544731)]</t>
+          <t>[np.float64(0.5083562277110025), np.float64(0.5058309297439733)]</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[0.5555555555555556]</t>
+          <t>[0.56, 0.552]</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1480,14 +1480,14 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0.538090032544731</v>
+        <v>0.5070935787274879</v>
       </c>
       <c r="F34" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.556</v>
       </c>
       <c r="G34" t="n">
         <v>7</v>
@@ -1527,12 +1527,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>[np.float64(0.6521265106560312), np.float64(0.6386810592005396)]</t>
+          <t>[np.float64(0.5374629936273772), np.float64(0.538090032544731)]</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[0.6904761904761905, 0.68]</t>
+          <t>[0.5476190476190477, 0.5555555555555556]</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1542,14 +1542,14 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-1.5-flash-001-finetuned</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0.6454037849282854</v>
+        <v>0.5377765130860541</v>
       </c>
       <c r="F36" t="n">
-        <v>0.6852380952380952</v>
+        <v>0.5515873015873016</v>
       </c>
       <c r="G36" t="n">
         <v>7</v>
@@ -1558,12 +1558,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>[np.float64(0.532920304983848)]</t>
+          <t>[np.float64(0.6524644518850284), np.float64(0.6482872200263505)]</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[0.5714285714285714]</t>
+          <t>[0.7073170731707317, 0.6942148760330579]</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1573,14 +1573,14 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0.532920304983848</v>
+        <v>0.6503758359556895</v>
       </c>
       <c r="F37" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.7007659746018948</v>
       </c>
       <c r="G37" t="n">
         <v>8</v>
@@ -1589,12 +1589,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>[np.float64(0.6524644518850284), np.float64(0.6482872200263505)]</t>
+          <t>[np.float64(0.4541337907375644), np.float64(0.47122859025032937)]</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[0.7073170731707317, 0.6942148760330579]</t>
+          <t>[0.52, 0.5317460317460317]</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1604,14 +1604,14 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0.6503758359556895</v>
+        <v>0.4626811904939468</v>
       </c>
       <c r="F38" t="n">
-        <v>0.7007659746018948</v>
+        <v>0.5258730158730158</v>
       </c>
       <c r="G38" t="n">
         <v>8</v>
@@ -1620,12 +1620,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>[np.float64(0.6562992627116154), np.float64(0.6445754716981131)]</t>
+          <t>[np.float64(0.5652965964746538), np.float64(0.532920304983848)]</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[0.696, 0.68]</t>
+          <t>[0.6190476190476191, 0.5714285714285714]</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1635,14 +1635,14 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-1.5-flash-001-finetuned</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.6504373672048642</v>
+        <v>0.549108450729251</v>
       </c>
       <c r="F39" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.5952380952380952</v>
       </c>
       <c r="G39" t="n">
         <v>8</v>
@@ -1651,12 +1651,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>[np.float64(0.5464676134142537), np.float64(0.5505998448192124)]</t>
+          <t>[np.float64(0.6562992627116154), np.float64(0.6445754716981131)]</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[0.6031746031746031, 0.6111111111111112]</t>
+          <t>[0.696, 0.68]</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1666,14 +1666,14 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>gemini-2.0-flash-exp</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0.548533729116733</v>
+        <v>0.6504373672048642</v>
       </c>
       <c r="F40" t="n">
-        <v>0.6071428571428572</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="G40" t="n">
         <v>8</v>
@@ -1682,12 +1682,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>[np.float64(0.4541337907375644), np.float64(0.47122859025032937)]</t>
+          <t>[np.float64(0.5464676134142537), np.float64(0.5505998448192124)]</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[0.52, 0.5317460317460317]</t>
+          <t>[0.6031746031746031, 0.6111111111111112]</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1697,14 +1697,14 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0.4626811904939468</v>
+        <v>0.548533729116733</v>
       </c>
       <c r="F41" t="n">
-        <v>0.5258730158730158</v>
+        <v>0.6071428571428572</v>
       </c>
       <c r="G41" t="n">
         <v>8</v>
@@ -1744,12 +1744,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>[np.float64(0.5361160714285714), np.float64(0.5477406704101712)]</t>
+          <t>[np.float64(0.6263474048099917), np.float64(0.6086457590876693)]</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[0.576, 0.5873015873015873]</t>
+          <t>[0.6829268292682927, 0.6693548387096774]</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1759,14 +1759,14 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.5419283709193713</v>
+        <v>0.6174965819488305</v>
       </c>
       <c r="F43" t="n">
-        <v>0.5816507936507936</v>
+        <v>0.6761408339889851</v>
       </c>
       <c r="G43" t="n">
         <v>9</v>
@@ -1775,12 +1775,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>[np.float64(0.6263474048099917), np.float64(0.6086457590876693)]</t>
+          <t>[np.float64(0.5313937481113387), np.float64(0.5716755601056871)]</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[0.6829268292682927, 0.6693548387096774]</t>
+          <t>[0.5634920634920635, 0.5873015873015873]</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1790,14 +1790,14 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-1.5-flash-001-finetuned</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0.6174965819488305</v>
+        <v>0.5515346541085129</v>
       </c>
       <c r="F44" t="n">
-        <v>0.6761408339889851</v>
+        <v>0.5753968253968254</v>
       </c>
       <c r="G44" t="n">
         <v>9</v>
@@ -1806,12 +1806,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>[np.float64(0.5313937481113387)]</t>
+          <t>[np.float64(0.6159932363750098), np.float64(0.5832183782005592)]</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[0.5634920634920635]</t>
+          <t>[0.6666666666666666, 0.6349206349206349]</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1821,14 +1821,14 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0.5313937481113387</v>
+        <v>0.5996058072877846</v>
       </c>
       <c r="F45" t="n">
-        <v>0.5634920634920635</v>
+        <v>0.6507936507936507</v>
       </c>
       <c r="G45" t="n">
         <v>9</v>
@@ -1837,12 +1837,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>[np.float64(0.6159932363750098), np.float64(0.5832183782005592)]</t>
+          <t>[np.float64(0.5361160714285714), np.float64(0.5477406704101712)]</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[0.6666666666666666, 0.6349206349206349]</t>
+          <t>[0.576, 0.5873015873015873]</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1852,14 +1852,14 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>gemini-2.0-flash-exp</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0.5996058072877846</v>
+        <v>0.5419283709193713</v>
       </c>
       <c r="F46" t="n">
-        <v>0.6507936507936507</v>
+        <v>0.5816507936507936</v>
       </c>
       <c r="G46" t="n">
         <v>9</v>
@@ -1868,12 +1868,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>[np.float64(0.6074765461770609), np.float64(0.5969074715487381)]</t>
+          <t>[np.float64(0.5203264226500969), np.float64(0.5445767195767196)]</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[0.656, 0.6585365853658537]</t>
+          <t>[0.5873015873015873, 0.5952380952380952]</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1883,14 +1883,14 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.6021920088628996</v>
+        <v>0.5324515711134082</v>
       </c>
       <c r="F47" t="n">
-        <v>0.6572682926829269</v>
+        <v>0.5912698412698413</v>
       </c>
       <c r="G47" t="n">
         <v>10</v>
@@ -1899,12 +1899,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>[np.float64(0.41419540229885055), np.float64(0.3414374445430346)]</t>
+          <t>[np.float64(0.5873665845648604), np.float64(0.5821868173138465)]</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[0.472, 0.4126984126984127]</t>
+          <t>[0.6333333333333333, 0.639344262295082]</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1914,14 +1914,14 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0.3778164234209426</v>
+        <v>0.5847767009393534</v>
       </c>
       <c r="F48" t="n">
-        <v>0.4423492063492063</v>
+        <v>0.6363387978142077</v>
       </c>
       <c r="G48" t="n">
         <v>10</v>
@@ -1930,12 +1930,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>[np.float64(0.5203264226500969), np.float64(0.5445767195767196)]</t>
+          <t>[np.float64(0.5447754984853544), np.float64(0.5002068881586954)]</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[0.5873015873015873, 0.5952380952380952]</t>
+          <t>[0.5793650793650794, 0.5396825396825397]</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1945,14 +1945,14 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>gemini-2.0-flash-exp</t>
+          <t>gemini-1.5-flash-001-finetuned</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0.5324515711134082</v>
+        <v>0.5224911933220249</v>
       </c>
       <c r="F49" t="n">
-        <v>0.5912698412698413</v>
+        <v>0.5595238095238095</v>
       </c>
       <c r="G49" t="n">
         <v>10</v>
@@ -1961,12 +1961,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>[np.float64(0.5873665845648604), np.float64(0.5821868173138465)]</t>
+          <t>[np.float64(0.6074765461770609), np.float64(0.5969074715487381)]</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[0.6333333333333333, 0.639344262295082]</t>
+          <t>[0.656, 0.6585365853658537]</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1976,14 +1976,14 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.5847767009393534</v>
+        <v>0.6021920088628996</v>
       </c>
       <c r="F50" t="n">
-        <v>0.6363387978142077</v>
+        <v>0.6572682926829269</v>
       </c>
       <c r="G50" t="n">
         <v>10</v>
@@ -1992,12 +1992,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>[np.float64(0.5447754984853544)]</t>
+          <t>[np.float64(0.41419540229885055), np.float64(0.3414374445430346)]</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[0.5793650793650794]</t>
+          <t>[0.472, 0.4126984126984127]</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2007,14 +2007,14 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>gemini-1.5-flash-001-tuning</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>0.5447754984853544</v>
+        <v>0.3778164234209426</v>
       </c>
       <c r="F51" t="n">
-        <v>0.5793650793650794</v>
+        <v>0.4423492063492063</v>
       </c>
       <c r="G51" t="n">
         <v>10</v>
@@ -2023,12 +2023,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>[np.float64(0.3380952380952381), np.float64(0.31666666666666665)]</t>
+          <t>[np.float64(0.4766586843438264), np.float64(0.48588209656103254)]</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[0.3333333333333333, 0.38461538461538464]</t>
+          <t>[0.5, 0.5238095238095238]</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2042,10 +2042,10 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>0.3273809523809524</v>
+        <v>0.4812703904524295</v>
       </c>
       <c r="F52" t="n">
-        <v>0.358974358974359</v>
+        <v>0.5119047619047619</v>
       </c>
       <c r="G52" t="n">
         <v>11</v>
@@ -2054,12 +2054,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>[np.float64(0.5237903225806451), np.float64(0.5487336811307223)]</t>
+          <t>[np.float64(0.590716894099558), np.float64(0.5747434017595308)]</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[0.5634920634920635, 0.5952380952380952]</t>
+          <t>[0.6428571428571429, 0.6349206349206349]</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2069,14 +2069,14 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>0.5362620018556836</v>
+        <v>0.5827301479295444</v>
       </c>
       <c r="F53" t="n">
-        <v>0.5793650793650793</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="G53" t="n">
         <v>11</v>
@@ -2085,12 +2085,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>[np.float64(0.6087991718426502), np.float64(0.5690200322553264)]</t>
+          <t>[np.float64(0.5160615200660967), np.float64(0.5104956066054465)]</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[0.6428571428571429, 0.6111111111111112]</t>
+          <t>[0.5714285714285714, 0.5634920634920635]</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2100,14 +2100,14 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>gemini-2.0-flash-exp</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>0.5889096020489883</v>
+        <v>0.5132785633357716</v>
       </c>
       <c r="F54" t="n">
-        <v>0.626984126984127</v>
+        <v>0.5674603174603174</v>
       </c>
       <c r="G54" t="n">
         <v>11</v>
@@ -2116,12 +2116,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>[np.float64(0.5236538107511046), np.float64(0.4968177855274629)]</t>
+          <t>[np.float64(0.49615630389258436), np.float64(0.508381806163761)]</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[0.5476190476190477, 0.5158730158730159]</t>
+          <t>[0.5238095238095238, 0.5317460317460317]</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2135,137 +2135,13 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>0.5102357981392838</v>
+        <v>0.5022690550281728</v>
       </c>
       <c r="F55" t="n">
-        <v>0.5317460317460319</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="G55" t="n">
         <v>11</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>[np.float64(0.49615630389258436), np.float64(0.508381806163761)]</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>[0.5238095238095238, 0.5317460317460317]</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>promptN12</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>claude-3-5-sonnet-20241022</t>
-        </is>
-      </c>
-      <c r="E56" t="n">
-        <v>0.5022690550281728</v>
-      </c>
-      <c r="F56" t="n">
-        <v>0.5277777777777778</v>
-      </c>
-      <c r="G56" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>[np.float64(0.590716894099558), np.float64(0.5747434017595308)]</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>[0.6428571428571429, 0.6349206349206349]</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>promptN12</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>gemini-2.0-flash-exp</t>
-        </is>
-      </c>
-      <c r="E57" t="n">
-        <v>0.5827301479295444</v>
-      </c>
-      <c r="F57" t="n">
-        <v>0.6388888888888888</v>
-      </c>
-      <c r="G57" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>[np.float64(0.48588209656103254), np.float64(0.4766586843438264)]</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>[0.5238095238095238, 0.5]</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>promptN12</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>gpt-4o</t>
-        </is>
-      </c>
-      <c r="E58" t="n">
-        <v>0.4812703904524295</v>
-      </c>
-      <c r="F58" t="n">
-        <v>0.5119047619047619</v>
-      </c>
-      <c r="G58" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>[np.float64(0.5160615200660967), np.float64(0.5104956066054465)]</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>[0.5714285714285714, 0.5634920634920635]</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>promptN12</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>gemini-1.5-pro</t>
-        </is>
-      </c>
-      <c r="E59" t="n">
-        <v>0.5132785633357716</v>
-      </c>
-      <c r="F59" t="n">
-        <v>0.5674603174603174</v>
-      </c>
-      <c r="G59" t="n">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>